<commit_message>
10x resuls and docs
</commit_message>
<xml_diff>
--- a/tgs_salt/avaliacao.xlsx
+++ b/tgs_salt/avaliacao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\_phd\code\textureSSD\tgs_salt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dados\0Code\textureSSD\tgs_salt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57709E9E-5C67-4269-A1E1-491FE7C8BD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0AFE99-D828-4C63-900E-67F06AA7147C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="18000" xr2:uid="{D7F9F861-84D9-46D0-A267-9E07DC75199E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D7F9F861-84D9-46D0-A267-9E07DC75199E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -161,16 +161,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,6 +186,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>96454</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47924</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B8EC3CF-BD7D-58FF-B7B5-E7FC3B6CC7E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9848850" y="3238500"/>
+          <a:ext cx="8630854" cy="2143424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>177075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>201792</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>143310</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1E67877-8CBE-1C2D-82CB-E824FC2660E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8972550" y="6273075"/>
+          <a:ext cx="11441292" cy="2823735"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -488,7 +581,7 @@
   <dimension ref="A3:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,11 +598,11 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
       <c r="H5" t="s">
         <v>17</v>
       </c>
@@ -538,272 +631,272 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0.92070428600119403</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.86979672033208699</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>0.88281612816329602</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="7">
+      <c r="F7" s="4"/>
+      <c r="G7" s="6">
         <v>0.93</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>0.89</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>2</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>0.96540345118519899</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.93017401337063799</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0.94457428051736503</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="7">
+      <c r="F8" s="4"/>
+      <c r="G8" s="6">
         <v>0.94</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>0.88</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>3</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.94205202427869195</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.93541959656268003</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>0.9386277495191</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4">
         <v>0.95</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>0.87</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>0.9</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>4</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>0.97736263736263695</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>0.86384666226040896</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>0.90961273205167903</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4">
         <v>0.97</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>0.92</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>0.94</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>5</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>0.79</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>0.827136728766794</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>0.81081145608399396</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4">
         <v>0.78</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>0.81</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>0.79</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>6</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>0.93</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>0.93</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>0.93</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8">
+      <c r="F12" s="7"/>
+      <c r="G12" s="7">
         <v>0.91</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <v>0.91</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <v>0.9</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>7</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>0.92</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>0.96</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>0.94</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8">
+      <c r="F13" s="7"/>
+      <c r="G13" s="7">
         <v>0.91</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>0.94</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>0.93</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>8</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>0.94</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>0.92</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>0.92</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8">
+      <c r="F14" s="7"/>
+      <c r="G14" s="7">
         <v>0.95</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <v>0.92</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <v>0.93</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>9</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>0.81</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>0.98</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>0.87</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8">
+      <c r="F15" s="7"/>
+      <c r="G15" s="7">
         <v>0.9</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="7">
         <v>0.99</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <v>0.94</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>10</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>0.9</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="8">
         <v>0.9</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>0.9</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8">
+      <c r="F16" s="7"/>
+      <c r="G16" s="7">
         <v>0.88</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <v>0.87</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="7">
         <v>0.87</v>
       </c>
     </row>
@@ -811,27 +904,27 @@
       <c r="B19" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <f>AVERAGE(C7:C16)</f>
         <v>0.90955223988277223</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <f>AVERAGE(D7:D16)</f>
         <v>0.91163737212926077</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <f>AVERAGE(E7:E16)</f>
         <v>0.90464423463354338</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <f>AVERAGE(G7:G16)</f>
         <v>0.91200000000000014</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="3">
         <f>AVERAGE(H7:H16)</f>
         <v>0.9</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="3">
         <f>AVERAGE(I7:I16)</f>
         <v>0.8999999999999998</v>
       </c>
@@ -919,7 +1012,7 @@
       <c r="E35" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="10">
+      <c r="J35" s="9">
         <v>1</v>
       </c>
     </row>
@@ -927,7 +1020,7 @@
       <c r="E36" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="10">
+      <c r="J36" s="9">
         <v>1</v>
       </c>
     </row>
@@ -948,5 +1041,6 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Trebuchet MS"&amp;9&amp;K737373PÚBLICA</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>